<commit_message>
Inhaltlich einheitliche Sortierung IG gICS
</commit_message>
<xml_diff>
--- a/output/StructureDefinition-ConsentModule.xlsx
+++ b/output/StructureDefinition-ConsentModule.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4383" uniqueCount="667">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4383" uniqueCount="666">
   <si>
     <t>Property</t>
   </si>
@@ -33,7 +33,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>2025.1.0</t>
+    <t>2025.2.0</t>
   </si>
   <si>
     <t>Name</t>
@@ -1687,7 +1687,7 @@
 </t>
   </si>
   <si>
-    <t>Text als Markdown</t>
+    <t>String equivalent with markdown</t>
   </si>
   <si>
     <t>This is an equivalent of the string on which the extension is sent, but includes additional markdown (see documentation about [markdown](http://hl7.org/fhir/R4/datatypes.html#markdown). Note that using HTML  [xhtml](http://hl7.org/fhir/R4/extension-rendering-xhtml.html) can allow for greater precision of display.</t>
@@ -1718,10 +1718,6 @@
   </si>
   <si>
     <t>Questionnaire.item.text.extension.value[x]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">type:$this}
-</t>
   </si>
   <si>
     <t>Questionnaire.item.text.extension:renderingMarkdown.value[x]:valueMarkdown</t>
@@ -12322,7 +12318,7 @@
         <v>530</v>
       </c>
       <c r="D97" t="s" s="2">
-        <v>102</v>
+        <v>21</v>
       </c>
       <c r="E97" s="2"/>
       <c r="F97" t="s" s="2">
@@ -12349,9 +12345,7 @@
       <c r="M97" t="s" s="2">
         <v>533</v>
       </c>
-      <c r="N97" t="s" s="2">
-        <v>106</v>
-      </c>
+      <c r="N97" s="2"/>
       <c r="O97" s="2"/>
       <c r="P97" t="s" s="2">
         <v>21</v>
@@ -12792,14 +12786,16 @@
         <v>21</v>
       </c>
       <c r="AB101" t="s" s="2">
-        <v>543</v>
-      </c>
-      <c r="AC101" s="2"/>
+        <v>21</v>
+      </c>
+      <c r="AC101" t="s" s="2">
+        <v>21</v>
+      </c>
       <c r="AD101" t="s" s="2">
         <v>21</v>
       </c>
       <c r="AE101" t="s" s="2">
-        <v>109</v>
+        <v>21</v>
       </c>
       <c r="AF101" t="s" s="2">
         <v>457</v>
@@ -12819,13 +12815,13 @@
     </row>
     <row r="102" hidden="true">
       <c r="A102" t="s" s="2">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="B102" t="s" s="2">
         <v>542</v>
       </c>
       <c r="C102" t="s" s="2">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="D102" t="s" s="2">
         <v>21</v>
@@ -12921,16 +12917,16 @@
     </row>
     <row r="103" hidden="true">
       <c r="A103" t="s" s="2">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="B103" t="s" s="2">
         <v>528</v>
       </c>
       <c r="C103" t="s" s="2">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="D103" t="s" s="2">
-        <v>102</v>
+        <v>21</v>
       </c>
       <c r="E103" s="2"/>
       <c r="F103" t="s" s="2">
@@ -12949,17 +12945,15 @@
         <v>21</v>
       </c>
       <c r="K103" t="s" s="2">
+        <v>547</v>
+      </c>
+      <c r="L103" t="s" s="2">
         <v>548</v>
       </c>
-      <c r="L103" t="s" s="2">
+      <c r="M103" t="s" s="2">
         <v>549</v>
       </c>
-      <c r="M103" t="s" s="2">
-        <v>550</v>
-      </c>
-      <c r="N103" t="s" s="2">
-        <v>106</v>
-      </c>
+      <c r="N103" s="2"/>
       <c r="O103" s="2"/>
       <c r="P103" t="s" s="2">
         <v>21</v>
@@ -13025,7 +13019,7 @@
     </row>
     <row r="104" hidden="true">
       <c r="A104" t="s" s="2">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="B104" t="s" s="2">
         <v>535</v>
@@ -13125,7 +13119,7 @@
     </row>
     <row r="105" hidden="true">
       <c r="A105" t="s" s="2">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="B105" t="s" s="2">
         <v>537</v>
@@ -13227,7 +13221,7 @@
     </row>
     <row r="106" hidden="true">
       <c r="A106" t="s" s="2">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="B106" t="s" s="2">
         <v>539</v>
@@ -13270,7 +13264,7 @@
       </c>
       <c r="Q106" s="2"/>
       <c r="R106" t="s" s="2">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="S106" t="s" s="2">
         <v>21</v>
@@ -13329,7 +13323,7 @@
     </row>
     <row r="107" hidden="true">
       <c r="A107" t="s" s="2">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="B107" t="s" s="2">
         <v>542</v>
@@ -13400,14 +13394,16 @@
         <v>21</v>
       </c>
       <c r="AB107" t="s" s="2">
-        <v>543</v>
-      </c>
-      <c r="AC107" s="2"/>
+        <v>21</v>
+      </c>
+      <c r="AC107" t="s" s="2">
+        <v>21</v>
+      </c>
       <c r="AD107" t="s" s="2">
         <v>21</v>
       </c>
       <c r="AE107" t="s" s="2">
-        <v>109</v>
+        <v>21</v>
       </c>
       <c r="AF107" t="s" s="2">
         <v>457</v>
@@ -13427,13 +13423,13 @@
     </row>
     <row r="108" hidden="true">
       <c r="A108" t="s" s="2">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="B108" t="s" s="2">
         <v>542</v>
       </c>
       <c r="C108" t="s" s="2">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="D108" t="s" s="2">
         <v>21</v>
@@ -13529,10 +13525,10 @@
     </row>
     <row r="109" hidden="true">
       <c r="A109" t="s" s="2">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="B109" t="s" s="2">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="C109" s="2"/>
       <c r="D109" t="s" s="2">
@@ -13558,10 +13554,10 @@
         <v>97</v>
       </c>
       <c r="L109" t="s" s="2">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="M109" t="s" s="2">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="N109" s="2"/>
       <c r="O109" s="2"/>
@@ -13585,34 +13581,34 @@
         <v>21</v>
       </c>
       <c r="W109" t="s" s="2">
+        <v>559</v>
+      </c>
+      <c r="X109" t="s" s="2">
+        <v>21</v>
+      </c>
+      <c r="Y109" t="s" s="2">
+        <v>21</v>
+      </c>
+      <c r="Z109" t="s" s="2">
+        <v>21</v>
+      </c>
+      <c r="AA109" t="s" s="2">
+        <v>21</v>
+      </c>
+      <c r="AB109" t="s" s="2">
+        <v>21</v>
+      </c>
+      <c r="AC109" t="s" s="2">
+        <v>21</v>
+      </c>
+      <c r="AD109" t="s" s="2">
+        <v>21</v>
+      </c>
+      <c r="AE109" t="s" s="2">
+        <v>21</v>
+      </c>
+      <c r="AF109" t="s" s="2">
         <v>560</v>
-      </c>
-      <c r="X109" t="s" s="2">
-        <v>21</v>
-      </c>
-      <c r="Y109" t="s" s="2">
-        <v>21</v>
-      </c>
-      <c r="Z109" t="s" s="2">
-        <v>21</v>
-      </c>
-      <c r="AA109" t="s" s="2">
-        <v>21</v>
-      </c>
-      <c r="AB109" t="s" s="2">
-        <v>21</v>
-      </c>
-      <c r="AC109" t="s" s="2">
-        <v>21</v>
-      </c>
-      <c r="AD109" t="s" s="2">
-        <v>21</v>
-      </c>
-      <c r="AE109" t="s" s="2">
-        <v>21</v>
-      </c>
-      <c r="AF109" t="s" s="2">
-        <v>561</v>
       </c>
       <c r="AG109" t="s" s="2">
         <v>75</v>
@@ -13629,10 +13625,10 @@
     </row>
     <row r="110">
       <c r="A110" t="s" s="2">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="B110" t="s" s="2">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="C110" s="2"/>
       <c r="D110" t="s" s="2">
@@ -13658,16 +13654,16 @@
         <v>163</v>
       </c>
       <c r="L110" t="s" s="2">
+        <v>562</v>
+      </c>
+      <c r="M110" t="s" s="2">
         <v>563</v>
       </c>
-      <c r="M110" t="s" s="2">
+      <c r="N110" t="s" s="2">
         <v>564</v>
       </c>
-      <c r="N110" t="s" s="2">
+      <c r="O110" t="s" s="2">
         <v>565</v>
-      </c>
-      <c r="O110" t="s" s="2">
-        <v>566</v>
       </c>
       <c r="P110" t="s" s="2">
         <v>21</v>
@@ -13695,11 +13691,11 @@
         <v>211</v>
       </c>
       <c r="Y110" t="s" s="2">
+        <v>566</v>
+      </c>
+      <c r="Z110" t="s" s="2">
         <v>567</v>
       </c>
-      <c r="Z110" t="s" s="2">
-        <v>568</v>
-      </c>
       <c r="AA110" t="s" s="2">
         <v>21</v>
       </c>
@@ -13716,7 +13712,7 @@
         <v>21</v>
       </c>
       <c r="AF110" t="s" s="2">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="AG110" t="s" s="2">
         <v>82</v>
@@ -13733,10 +13729,10 @@
     </row>
     <row r="111" hidden="true">
       <c r="A111" t="s" s="2">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="B111" t="s" s="2">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="C111" s="2"/>
       <c r="D111" t="s" s="2">
@@ -13762,16 +13758,16 @@
         <v>422</v>
       </c>
       <c r="L111" t="s" s="2">
+        <v>569</v>
+      </c>
+      <c r="M111" t="s" s="2">
         <v>570</v>
       </c>
-      <c r="M111" t="s" s="2">
+      <c r="N111" t="s" s="2">
         <v>571</v>
       </c>
-      <c r="N111" t="s" s="2">
+      <c r="O111" t="s" s="2">
         <v>572</v>
-      </c>
-      <c r="O111" t="s" s="2">
-        <v>573</v>
       </c>
       <c r="P111" t="s" s="2">
         <v>21</v>
@@ -13820,7 +13816,7 @@
         <v>21</v>
       </c>
       <c r="AF111" t="s" s="2">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="AG111" t="s" s="2">
         <v>75</v>
@@ -13832,15 +13828,15 @@
         <v>94</v>
       </c>
       <c r="AJ111" t="s" s="2">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="112" hidden="true">
       <c r="A112" t="s" s="2">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="B112" t="s" s="2">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="C112" s="2"/>
       <c r="D112" t="s" s="2">
@@ -13937,10 +13933,10 @@
     </row>
     <row r="113" hidden="true">
       <c r="A113" t="s" s="2">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="B113" t="s" s="2">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="C113" s="2"/>
       <c r="D113" t="s" s="2">
@@ -14039,10 +14035,10 @@
     </row>
     <row r="114" hidden="true">
       <c r="A114" t="s" s="2">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B114" t="s" s="2">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="C114" s="2"/>
       <c r="D114" t="s" s="2">
@@ -14143,10 +14139,10 @@
     </row>
     <row r="115" hidden="true">
       <c r="A115" t="s" s="2">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="B115" t="s" s="2">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="C115" s="2"/>
       <c r="D115" t="s" s="2">
@@ -14172,13 +14168,13 @@
         <v>97</v>
       </c>
       <c r="L115" t="s" s="2">
+        <v>578</v>
+      </c>
+      <c r="M115" t="s" s="2">
         <v>579</v>
       </c>
-      <c r="M115" t="s" s="2">
+      <c r="N115" t="s" s="2">
         <v>580</v>
-      </c>
-      <c r="N115" t="s" s="2">
-        <v>581</v>
       </c>
       <c r="O115" s="2"/>
       <c r="P115" t="s" s="2">
@@ -14228,7 +14224,7 @@
         <v>21</v>
       </c>
       <c r="AF115" t="s" s="2">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="AG115" t="s" s="2">
         <v>82</v>
@@ -14245,10 +14241,10 @@
     </row>
     <row r="116" hidden="true">
       <c r="A116" t="s" s="2">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="B116" t="s" s="2">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="C116" s="2"/>
       <c r="D116" t="s" s="2">
@@ -14274,10 +14270,10 @@
         <v>163</v>
       </c>
       <c r="L116" t="s" s="2">
+        <v>582</v>
+      </c>
+      <c r="M116" t="s" s="2">
         <v>583</v>
-      </c>
-      <c r="M116" t="s" s="2">
-        <v>584</v>
       </c>
       <c r="N116" t="s" s="2">
         <v>340</v>
@@ -14309,11 +14305,11 @@
         <v>211</v>
       </c>
       <c r="Y116" t="s" s="2">
+        <v>584</v>
+      </c>
+      <c r="Z116" t="s" s="2">
         <v>585</v>
       </c>
-      <c r="Z116" t="s" s="2">
-        <v>586</v>
-      </c>
       <c r="AA116" t="s" s="2">
         <v>21</v>
       </c>
@@ -14330,7 +14326,7 @@
         <v>21</v>
       </c>
       <c r="AF116" t="s" s="2">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="AG116" t="s" s="2">
         <v>82</v>
@@ -14347,10 +14343,10 @@
     </row>
     <row r="117" hidden="true">
       <c r="A117" t="s" s="2">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="B117" t="s" s="2">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="C117" s="2"/>
       <c r="D117" t="s" s="2">
@@ -14373,13 +14369,13 @@
         <v>21</v>
       </c>
       <c r="K117" t="s" s="2">
+        <v>587</v>
+      </c>
+      <c r="L117" t="s" s="2">
         <v>588</v>
       </c>
-      <c r="L117" t="s" s="2">
+      <c r="M117" t="s" s="2">
         <v>589</v>
-      </c>
-      <c r="M117" t="s" s="2">
-        <v>590</v>
       </c>
       <c r="N117" s="2"/>
       <c r="O117" s="2"/>
@@ -14409,37 +14405,37 @@
         <v>153</v>
       </c>
       <c r="Y117" t="s" s="2">
+        <v>590</v>
+      </c>
+      <c r="Z117" t="s" s="2">
         <v>591</v>
       </c>
-      <c r="Z117" t="s" s="2">
+      <c r="AA117" t="s" s="2">
+        <v>21</v>
+      </c>
+      <c r="AB117" t="s" s="2">
+        <v>21</v>
+      </c>
+      <c r="AC117" t="s" s="2">
+        <v>21</v>
+      </c>
+      <c r="AD117" t="s" s="2">
+        <v>21</v>
+      </c>
+      <c r="AE117" t="s" s="2">
+        <v>21</v>
+      </c>
+      <c r="AF117" t="s" s="2">
+        <v>586</v>
+      </c>
+      <c r="AG117" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AH117" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AI117" t="s" s="2">
         <v>592</v>
-      </c>
-      <c r="AA117" t="s" s="2">
-        <v>21</v>
-      </c>
-      <c r="AB117" t="s" s="2">
-        <v>21</v>
-      </c>
-      <c r="AC117" t="s" s="2">
-        <v>21</v>
-      </c>
-      <c r="AD117" t="s" s="2">
-        <v>21</v>
-      </c>
-      <c r="AE117" t="s" s="2">
-        <v>21</v>
-      </c>
-      <c r="AF117" t="s" s="2">
-        <v>587</v>
-      </c>
-      <c r="AG117" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="AH117" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="AI117" t="s" s="2">
-        <v>593</v>
       </c>
       <c r="AJ117" t="s" s="2">
         <v>95</v>
@@ -14447,10 +14443,10 @@
     </row>
     <row r="118" hidden="true">
       <c r="A118" t="s" s="2">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="B118" t="s" s="2">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="C118" s="2"/>
       <c r="D118" t="s" s="2">
@@ -14476,13 +14472,13 @@
         <v>163</v>
       </c>
       <c r="L118" t="s" s="2">
+        <v>594</v>
+      </c>
+      <c r="M118" t="s" s="2">
         <v>595</v>
       </c>
-      <c r="M118" t="s" s="2">
+      <c r="N118" t="s" s="2">
         <v>596</v>
-      </c>
-      <c r="N118" t="s" s="2">
-        <v>597</v>
       </c>
       <c r="O118" s="2"/>
       <c r="P118" t="s" s="2">
@@ -14511,37 +14507,37 @@
         <v>211</v>
       </c>
       <c r="Y118" t="s" s="2">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="Z118" t="s" s="2">
+        <v>597</v>
+      </c>
+      <c r="AA118" t="s" s="2">
+        <v>21</v>
+      </c>
+      <c r="AB118" t="s" s="2">
+        <v>21</v>
+      </c>
+      <c r="AC118" t="s" s="2">
+        <v>21</v>
+      </c>
+      <c r="AD118" t="s" s="2">
+        <v>21</v>
+      </c>
+      <c r="AE118" t="s" s="2">
+        <v>21</v>
+      </c>
+      <c r="AF118" t="s" s="2">
+        <v>593</v>
+      </c>
+      <c r="AG118" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AH118" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AI118" t="s" s="2">
         <v>598</v>
-      </c>
-      <c r="AA118" t="s" s="2">
-        <v>21</v>
-      </c>
-      <c r="AB118" t="s" s="2">
-        <v>21</v>
-      </c>
-      <c r="AC118" t="s" s="2">
-        <v>21</v>
-      </c>
-      <c r="AD118" t="s" s="2">
-        <v>21</v>
-      </c>
-      <c r="AE118" t="s" s="2">
-        <v>21</v>
-      </c>
-      <c r="AF118" t="s" s="2">
-        <v>594</v>
-      </c>
-      <c r="AG118" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="AH118" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="AI118" t="s" s="2">
-        <v>599</v>
       </c>
       <c r="AJ118" t="s" s="2">
         <v>95</v>
@@ -14549,10 +14545,10 @@
     </row>
     <row r="119" hidden="true">
       <c r="A119" t="s" s="2">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="B119" t="s" s="2">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="C119" s="2"/>
       <c r="D119" t="s" s="2">
@@ -14578,74 +14574,74 @@
         <v>278</v>
       </c>
       <c r="L119" t="s" s="2">
+        <v>600</v>
+      </c>
+      <c r="M119" t="s" s="2">
         <v>601</v>
       </c>
-      <c r="M119" t="s" s="2">
+      <c r="N119" t="s" s="2">
         <v>602</v>
-      </c>
-      <c r="N119" t="s" s="2">
-        <v>603</v>
       </c>
       <c r="O119" s="2"/>
       <c r="P119" t="s" s="2">
         <v>21</v>
       </c>
       <c r="Q119" t="s" s="2">
+        <v>603</v>
+      </c>
+      <c r="R119" t="s" s="2">
+        <v>21</v>
+      </c>
+      <c r="S119" t="s" s="2">
+        <v>21</v>
+      </c>
+      <c r="T119" t="s" s="2">
+        <v>21</v>
+      </c>
+      <c r="U119" t="s" s="2">
+        <v>21</v>
+      </c>
+      <c r="V119" t="s" s="2">
+        <v>21</v>
+      </c>
+      <c r="W119" t="s" s="2">
+        <v>21</v>
+      </c>
+      <c r="X119" t="s" s="2">
+        <v>21</v>
+      </c>
+      <c r="Y119" t="s" s="2">
+        <v>21</v>
+      </c>
+      <c r="Z119" t="s" s="2">
+        <v>21</v>
+      </c>
+      <c r="AA119" t="s" s="2">
+        <v>21</v>
+      </c>
+      <c r="AB119" t="s" s="2">
+        <v>21</v>
+      </c>
+      <c r="AC119" t="s" s="2">
+        <v>21</v>
+      </c>
+      <c r="AD119" t="s" s="2">
+        <v>21</v>
+      </c>
+      <c r="AE119" t="s" s="2">
+        <v>21</v>
+      </c>
+      <c r="AF119" t="s" s="2">
+        <v>599</v>
+      </c>
+      <c r="AG119" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AH119" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AI119" t="s" s="2">
         <v>604</v>
-      </c>
-      <c r="R119" t="s" s="2">
-        <v>21</v>
-      </c>
-      <c r="S119" t="s" s="2">
-        <v>21</v>
-      </c>
-      <c r="T119" t="s" s="2">
-        <v>21</v>
-      </c>
-      <c r="U119" t="s" s="2">
-        <v>21</v>
-      </c>
-      <c r="V119" t="s" s="2">
-        <v>21</v>
-      </c>
-      <c r="W119" t="s" s="2">
-        <v>21</v>
-      </c>
-      <c r="X119" t="s" s="2">
-        <v>21</v>
-      </c>
-      <c r="Y119" t="s" s="2">
-        <v>21</v>
-      </c>
-      <c r="Z119" t="s" s="2">
-        <v>21</v>
-      </c>
-      <c r="AA119" t="s" s="2">
-        <v>21</v>
-      </c>
-      <c r="AB119" t="s" s="2">
-        <v>21</v>
-      </c>
-      <c r="AC119" t="s" s="2">
-        <v>21</v>
-      </c>
-      <c r="AD119" t="s" s="2">
-        <v>21</v>
-      </c>
-      <c r="AE119" t="s" s="2">
-        <v>21</v>
-      </c>
-      <c r="AF119" t="s" s="2">
-        <v>600</v>
-      </c>
-      <c r="AG119" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="AH119" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="AI119" t="s" s="2">
-        <v>605</v>
       </c>
       <c r="AJ119" t="s" s="2">
         <v>95</v>
@@ -14653,10 +14649,10 @@
     </row>
     <row r="120" hidden="true">
       <c r="A120" t="s" s="2">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="B120" t="s" s="2">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="C120" s="2"/>
       <c r="D120" t="s" s="2">
@@ -14682,23 +14678,23 @@
         <v>278</v>
       </c>
       <c r="L120" t="s" s="2">
+        <v>606</v>
+      </c>
+      <c r="M120" t="s" s="2">
         <v>607</v>
       </c>
-      <c r="M120" t="s" s="2">
+      <c r="N120" t="s" s="2">
         <v>608</v>
       </c>
-      <c r="N120" t="s" s="2">
+      <c r="O120" t="s" s="2">
         <v>609</v>
       </c>
-      <c r="O120" t="s" s="2">
+      <c r="P120" t="s" s="2">
+        <v>21</v>
+      </c>
+      <c r="Q120" t="s" s="2">
         <v>610</v>
       </c>
-      <c r="P120" t="s" s="2">
-        <v>21</v>
-      </c>
-      <c r="Q120" t="s" s="2">
-        <v>611</v>
-      </c>
       <c r="R120" t="s" s="2">
         <v>21</v>
       </c>
@@ -14742,7 +14738,7 @@
         <v>21</v>
       </c>
       <c r="AF120" t="s" s="2">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="AG120" t="s" s="2">
         <v>75</v>
@@ -14751,7 +14747,7 @@
         <v>82</v>
       </c>
       <c r="AI120" t="s" s="2">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="AJ120" t="s" s="2">
         <v>95</v>
@@ -14759,10 +14755,10 @@
     </row>
     <row r="121" hidden="true">
       <c r="A121" t="s" s="2">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="B121" t="s" s="2">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="C121" s="2"/>
       <c r="D121" t="s" s="2">
@@ -14788,16 +14784,16 @@
         <v>278</v>
       </c>
       <c r="L121" t="s" s="2">
+        <v>612</v>
+      </c>
+      <c r="M121" t="s" s="2">
         <v>613</v>
       </c>
-      <c r="M121" t="s" s="2">
+      <c r="N121" t="s" s="2">
         <v>614</v>
       </c>
-      <c r="N121" t="s" s="2">
+      <c r="O121" t="s" s="2">
         <v>615</v>
-      </c>
-      <c r="O121" t="s" s="2">
-        <v>616</v>
       </c>
       <c r="P121" t="s" s="2">
         <v>21</v>
@@ -14846,7 +14842,7 @@
         <v>21</v>
       </c>
       <c r="AF121" t="s" s="2">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="AG121" t="s" s="2">
         <v>75</v>
@@ -14855,7 +14851,7 @@
         <v>82</v>
       </c>
       <c r="AI121" t="s" s="2">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="AJ121" t="s" s="2">
         <v>95</v>
@@ -14863,10 +14859,10 @@
     </row>
     <row r="122" hidden="true">
       <c r="A122" t="s" s="2">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="B122" t="s" s="2">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="C122" s="2"/>
       <c r="D122" t="s" s="2">
@@ -14889,16 +14885,16 @@
         <v>21</v>
       </c>
       <c r="K122" t="s" s="2">
+        <v>618</v>
+      </c>
+      <c r="L122" t="s" s="2">
         <v>619</v>
       </c>
-      <c r="L122" t="s" s="2">
+      <c r="M122" t="s" s="2">
         <v>620</v>
       </c>
-      <c r="M122" t="s" s="2">
+      <c r="N122" t="s" s="2">
         <v>621</v>
-      </c>
-      <c r="N122" t="s" s="2">
-        <v>622</v>
       </c>
       <c r="O122" s="2"/>
       <c r="P122" t="s" s="2">
@@ -14948,7 +14944,7 @@
         <v>21</v>
       </c>
       <c r="AF122" t="s" s="2">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="AG122" t="s" s="2">
         <v>75</v>
@@ -14957,7 +14953,7 @@
         <v>82</v>
       </c>
       <c r="AI122" t="s" s="2">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="AJ122" t="s" s="2">
         <v>95</v>
@@ -14965,10 +14961,10 @@
     </row>
     <row r="123" hidden="true">
       <c r="A123" t="s" s="2">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="B123" t="s" s="2">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="C123" s="2"/>
       <c r="D123" t="s" s="2">
@@ -14991,16 +14987,16 @@
         <v>21</v>
       </c>
       <c r="K123" t="s" s="2">
+        <v>624</v>
+      </c>
+      <c r="L123" t="s" s="2">
         <v>625</v>
       </c>
-      <c r="L123" t="s" s="2">
+      <c r="M123" t="s" s="2">
         <v>626</v>
       </c>
-      <c r="M123" t="s" s="2">
+      <c r="N123" t="s" s="2">
         <v>627</v>
-      </c>
-      <c r="N123" t="s" s="2">
-        <v>628</v>
       </c>
       <c r="O123" s="2"/>
       <c r="P123" t="s" s="2">
@@ -15050,7 +15046,7 @@
         <v>21</v>
       </c>
       <c r="AF123" t="s" s="2">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="AG123" t="s" s="2">
         <v>75</v>
@@ -15059,7 +15055,7 @@
         <v>82</v>
       </c>
       <c r="AI123" t="s" s="2">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="AJ123" t="s" s="2">
         <v>95</v>
@@ -15067,10 +15063,10 @@
     </row>
     <row r="124" hidden="true">
       <c r="A124" t="s" s="2">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="B124" t="s" s="2">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="C124" s="2"/>
       <c r="D124" t="s" s="2">
@@ -15096,13 +15092,13 @@
         <v>422</v>
       </c>
       <c r="L124" t="s" s="2">
+        <v>630</v>
+      </c>
+      <c r="M124" t="s" s="2">
         <v>631</v>
       </c>
-      <c r="M124" t="s" s="2">
+      <c r="N124" t="s" s="2">
         <v>632</v>
-      </c>
-      <c r="N124" t="s" s="2">
-        <v>633</v>
       </c>
       <c r="O124" s="2"/>
       <c r="P124" t="s" s="2">
@@ -15152,7 +15148,7 @@
         <v>21</v>
       </c>
       <c r="AF124" t="s" s="2">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="AG124" t="s" s="2">
         <v>75</v>
@@ -15161,7 +15157,7 @@
         <v>76</v>
       </c>
       <c r="AI124" t="s" s="2">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="AJ124" t="s" s="2">
         <v>95</v>
@@ -15169,10 +15165,10 @@
     </row>
     <row r="125" hidden="true">
       <c r="A125" t="s" s="2">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="B125" t="s" s="2">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="C125" s="2"/>
       <c r="D125" t="s" s="2">
@@ -15269,10 +15265,10 @@
     </row>
     <row r="126" hidden="true">
       <c r="A126" t="s" s="2">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="B126" t="s" s="2">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="C126" s="2"/>
       <c r="D126" t="s" s="2">
@@ -15371,10 +15367,10 @@
     </row>
     <row r="127" hidden="true">
       <c r="A127" t="s" s="2">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="B127" t="s" s="2">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="C127" s="2"/>
       <c r="D127" t="s" s="2">
@@ -15475,10 +15471,10 @@
     </row>
     <row r="128" hidden="true">
       <c r="A128" t="s" s="2">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="B128" t="s" s="2">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="C128" s="2"/>
       <c r="D128" t="s" s="2">
@@ -15501,16 +15497,16 @@
         <v>21</v>
       </c>
       <c r="K128" t="s" s="2">
+        <v>637</v>
+      </c>
+      <c r="L128" t="s" s="2">
         <v>638</v>
       </c>
-      <c r="L128" t="s" s="2">
+      <c r="M128" t="s" s="2">
         <v>639</v>
       </c>
-      <c r="M128" t="s" s="2">
+      <c r="N128" t="s" s="2">
         <v>640</v>
-      </c>
-      <c r="N128" t="s" s="2">
-        <v>641</v>
       </c>
       <c r="O128" s="2"/>
       <c r="P128" t="s" s="2">
@@ -15539,11 +15535,11 @@
         <v>153</v>
       </c>
       <c r="Y128" t="s" s="2">
+        <v>590</v>
+      </c>
+      <c r="Z128" t="s" s="2">
         <v>591</v>
       </c>
-      <c r="Z128" t="s" s="2">
-        <v>592</v>
-      </c>
       <c r="AA128" t="s" s="2">
         <v>21</v>
       </c>
@@ -15560,7 +15556,7 @@
         <v>21</v>
       </c>
       <c r="AF128" t="s" s="2">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="AG128" t="s" s="2">
         <v>82</v>
@@ -15577,10 +15573,10 @@
     </row>
     <row r="129" hidden="true">
       <c r="A129" t="s" s="2">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="B129" t="s" s="2">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="C129" s="2"/>
       <c r="D129" t="s" s="2">
@@ -15606,20 +15602,20 @@
         <v>278</v>
       </c>
       <c r="L129" t="s" s="2">
+        <v>642</v>
+      </c>
+      <c r="M129" t="s" s="2">
         <v>643</v>
       </c>
-      <c r="M129" t="s" s="2">
+      <c r="N129" t="s" s="2">
         <v>644</v>
-      </c>
-      <c r="N129" t="s" s="2">
-        <v>645</v>
       </c>
       <c r="O129" s="2"/>
       <c r="P129" t="s" s="2">
         <v>21</v>
       </c>
       <c r="Q129" t="s" s="2">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="R129" t="s" s="2">
         <v>21</v>
@@ -15664,7 +15660,7 @@
         <v>21</v>
       </c>
       <c r="AF129" t="s" s="2">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="AG129" t="s" s="2">
         <v>75</v>
@@ -15681,10 +15677,10 @@
     </row>
     <row r="130" hidden="true">
       <c r="A130" t="s" s="2">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="B130" t="s" s="2">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="C130" s="2"/>
       <c r="D130" t="s" s="2">
@@ -15710,16 +15706,16 @@
         <v>422</v>
       </c>
       <c r="L130" t="s" s="2">
+        <v>647</v>
+      </c>
+      <c r="M130" t="s" s="2">
         <v>648</v>
       </c>
-      <c r="M130" t="s" s="2">
+      <c r="N130" t="s" s="2">
         <v>649</v>
       </c>
-      <c r="N130" t="s" s="2">
+      <c r="O130" t="s" s="2">
         <v>650</v>
-      </c>
-      <c r="O130" t="s" s="2">
-        <v>651</v>
       </c>
       <c r="P130" t="s" s="2">
         <v>21</v>
@@ -15768,7 +15764,7 @@
         <v>21</v>
       </c>
       <c r="AF130" t="s" s="2">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="AG130" t="s" s="2">
         <v>75</v>
@@ -15777,7 +15773,7 @@
         <v>76</v>
       </c>
       <c r="AI130" t="s" s="2">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="AJ130" t="s" s="2">
         <v>95</v>
@@ -15785,10 +15781,10 @@
     </row>
     <row r="131" hidden="true">
       <c r="A131" t="s" s="2">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="B131" t="s" s="2">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="C131" s="2"/>
       <c r="D131" t="s" s="2">
@@ -15885,10 +15881,10 @@
     </row>
     <row r="132" hidden="true">
       <c r="A132" t="s" s="2">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="B132" t="s" s="2">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="C132" s="2"/>
       <c r="D132" t="s" s="2">
@@ -15987,10 +15983,10 @@
     </row>
     <row r="133" hidden="true">
       <c r="A133" t="s" s="2">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="B133" t="s" s="2">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="C133" s="2"/>
       <c r="D133" t="s" s="2">
@@ -16091,10 +16087,10 @@
     </row>
     <row r="134" hidden="true">
       <c r="A134" t="s" s="2">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="B134" t="s" s="2">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="C134" s="2"/>
       <c r="D134" t="s" s="2">
@@ -16117,16 +16113,16 @@
         <v>21</v>
       </c>
       <c r="K134" t="s" s="2">
+        <v>656</v>
+      </c>
+      <c r="L134" t="s" s="2">
         <v>657</v>
       </c>
-      <c r="L134" t="s" s="2">
+      <c r="M134" t="s" s="2">
         <v>658</v>
       </c>
-      <c r="M134" t="s" s="2">
+      <c r="N134" t="s" s="2">
         <v>659</v>
-      </c>
-      <c r="N134" t="s" s="2">
-        <v>660</v>
       </c>
       <c r="O134" s="2"/>
       <c r="P134" t="s" s="2">
@@ -16155,11 +16151,11 @@
         <v>153</v>
       </c>
       <c r="Y134" t="s" s="2">
+        <v>590</v>
+      </c>
+      <c r="Z134" t="s" s="2">
         <v>591</v>
       </c>
-      <c r="Z134" t="s" s="2">
-        <v>592</v>
-      </c>
       <c r="AA134" t="s" s="2">
         <v>21</v>
       </c>
@@ -16176,7 +16172,7 @@
         <v>21</v>
       </c>
       <c r="AF134" t="s" s="2">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="AG134" t="s" s="2">
         <v>82</v>
@@ -16193,10 +16189,10 @@
     </row>
     <row r="135" hidden="true">
       <c r="A135" t="s" s="2">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="B135" t="s" s="2">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="C135" s="2"/>
       <c r="D135" t="s" s="2">
@@ -16222,16 +16218,16 @@
         <v>21</v>
       </c>
       <c r="L135" t="s" s="2">
+        <v>661</v>
+      </c>
+      <c r="M135" t="s" s="2">
         <v>662</v>
       </c>
-      <c r="M135" t="s" s="2">
+      <c r="N135" t="s" s="2">
         <v>663</v>
       </c>
-      <c r="N135" t="s" s="2">
+      <c r="O135" t="s" s="2">
         <v>664</v>
-      </c>
-      <c r="O135" t="s" s="2">
-        <v>665</v>
       </c>
       <c r="P135" t="s" s="2">
         <v>21</v>
@@ -16280,7 +16276,7 @@
         <v>21</v>
       </c>
       <c r="AF135" t="s" s="2">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="AG135" t="s" s="2">
         <v>75</v>
@@ -16289,7 +16285,7 @@
         <v>76</v>
       </c>
       <c r="AI135" t="s" s="2">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="AJ135" t="s" s="2">
         <v>21</v>

</xml_diff>